<commit_message>
Re-add support for page break move and fix test
</commit_message>
<xml_diff>
--- a/test/templates/test-movePageBreakOption.xlsx
+++ b/test/templates/test-movePageBreakOption.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tmp\surveaexcel\NEWER\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neuhaeusser\Documents\aws\projects\forks\xlsx-template\test\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{53DAD8BB-6915-47EF-9A33-89F6E2A02814}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BED344-9DCB-4BD5-8AEF-A870E18D234B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="15840" windowWidth="29040" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" r:id="rId1" sheetId="1"/>
+    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName localSheetId="0" name="_xlnm.Print_Area">Feuil1!$A$1:$J$12</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$J$12</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,13 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>${table:myarray.name}</t>
-  </si>
-  <si>
-    <t>${name}</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>END</t>
   </si>
@@ -51,13 +45,16 @@
     <t>test</t>
   </si>
   <si>
-    <t>foo</t>
-  </si>
-  <si>
-    <t>john</t>
-  </si>
-  <si>
-    <t>doe</t>
+    <t>Spalte1</t>
+  </si>
+  <si>
+    <t>Spalte2</t>
+  </si>
+  <si>
+    <t>${table:users.name}</t>
+  </si>
+  <si>
+    <t>${table:users.surname}</t>
   </si>
 </sst>
 </file>
@@ -81,7 +78,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -141,12 +138,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -156,12 +169,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -172,6 +230,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{17D6E266-5EE9-47F5-B9C1-430D542E60FB}" name="Users" displayName="Users" ref="C4:D5" totalsRowShown="0" tableBorderDxfId="2">
+  <autoFilter ref="C4:D5" xr:uid="{17D6E266-5EE9-47F5-B9C1-430D542E60FB}"/>
+  <tableColumns count="2">
+    <tableColumn id="2" xr3:uid="{DCF73977-CA8E-4010-BF21-9C3A03A1EBBB}" name="Spalte1" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{B0BEA502-C70C-41EA-A205-9C593BF0DD3A}" name="Spalte2" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -436,71 +505,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" workbookViewId="0" zoomScale="160" zoomScaleNormal="100" zoomScaleSheetLayoutView="160">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="160" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B4" s="8"/>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="3"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B5" s="7"/>
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3"/>
-      <c r="F4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="4"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="3"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="3"/>
-      <c r="F5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="4"/>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="3"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
-      <c r="F6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
         <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="111">
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
+  <mergeCells count="1">
     <mergeCell ref="B6:D6"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" paperSize="9" r:id="rId1" scale="95" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="95" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>